<commit_message>
udpate cnn: add loss in excel
</commit_message>
<xml_diff>
--- a/conv_accuracies.xlsx
+++ b/conv_accuracies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,16 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Train Loss</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Test Loss</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Accuracy</t>
         </is>
       </c>
@@ -450,7 +460,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>42.0235</v>
+        <v>1.6553</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.4902</v>
+      </c>
+      <c r="D2" t="n">
+        <v>46.0594</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +474,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>48.8956</v>
+        <v>1.4175</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.3641</v>
+      </c>
+      <c r="D3" t="n">
+        <v>49.9046</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +488,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>49.9046</v>
+        <v>1.3171</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.2835</v>
+      </c>
+      <c r="D4" t="n">
+        <v>52.0862</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +502,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>52.168</v>
+        <v>1.2559</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.2457</v>
+      </c>
+      <c r="D5" t="n">
+        <v>53.1497</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +516,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>52.8225</v>
+        <v>1.2144</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.2281</v>
+      </c>
+      <c r="D6" t="n">
+        <v>53.9951</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +530,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>53.886</v>
+        <v>1.1906</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.207</v>
+      </c>
+      <c r="D7" t="n">
+        <v>53.8042</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +544,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>54.7041</v>
+        <v>1.1697</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.1787</v>
+      </c>
+      <c r="D8" t="n">
+        <v>56.204</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +558,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>54.186</v>
+        <v>1.1571</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.1751</v>
+      </c>
+      <c r="D9" t="n">
+        <v>55.0586</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +572,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>55.0859</v>
+        <v>1.1491</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1.1693</v>
+      </c>
+      <c r="D10" t="n">
+        <v>55.6586</v>
       </c>
     </row>
     <row r="11">
@@ -522,87 +586,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>55.195</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>55.8495</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>55.0314</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>54.5405</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>55.7404</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>55.4677</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
-        <v>55.3859</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>54.9768</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>55.8222</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="n">
-        <v>55.3586</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n">
-        <v>54.7587</v>
+        <v>1.1432</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.1663</v>
+      </c>
+      <c r="D11" t="n">
+        <v>55.3313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>